<commit_message>
s2t genai sql working
</commit_message>
<xml_diff>
--- a/datf_core/test/testprotocol/testselection_template.xlsx
+++ b/datf_core/test/testprotocol/testselection_template.xlsx
@@ -1485,7 +1485,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -3314,7 +3314,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
clean reports demo ready
</commit_message>
<xml_diff>
--- a/datf_core/test/testprotocol/testselection_template.xlsx
+++ b/datf_core/test/testprotocol/testselection_template.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI31"/>
+  <dimension ref="A1:AJ32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -699,6 +699,11 @@
       <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>samplelimit</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>dataprofilelimit</t>
         </is>
       </c>
     </row>
@@ -764,6 +769,9 @@
       <c r="AI2" t="n">
         <v>5</v>
       </c>
+      <c r="AJ2" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -827,6 +835,9 @@
       <c r="AI3" t="n">
         <v>5</v>
       </c>
+      <c r="AJ3" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -890,6 +901,9 @@
       <c r="AI4" t="n">
         <v>5</v>
       </c>
+      <c r="AJ4" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -953,6 +967,9 @@
       <c r="AI5" t="n">
         <v>5</v>
       </c>
+      <c r="AJ5" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1016,6 +1033,9 @@
       <c r="AI6" t="n">
         <v>5</v>
       </c>
+      <c r="AJ6" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1079,6 +1099,9 @@
       <c r="AI7" t="n">
         <v>5</v>
       </c>
+      <c r="AJ7" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1142,6 +1165,9 @@
       <c r="AI8" t="n">
         <v>5</v>
       </c>
+      <c r="AJ8" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1205,6 +1231,9 @@
       <c r="AI9" t="n">
         <v>5</v>
       </c>
+      <c r="AJ9" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1272,6 +1301,9 @@
       <c r="AI10" t="n">
         <v>8</v>
       </c>
+      <c r="AJ10" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1335,6 +1367,9 @@
       <c r="AI11" t="n">
         <v>5</v>
       </c>
+      <c r="AJ11" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1474,6 +1509,9 @@
       <c r="AI12" t="n">
         <v>5</v>
       </c>
+      <c r="AJ12" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1485,7 +1523,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1608,6 +1646,9 @@
       </c>
       <c r="AI13" t="n">
         <v>8</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="14">
@@ -1748,6 +1789,9 @@
       <c r="AI14" t="n">
         <v>5</v>
       </c>
+      <c r="AJ14" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1886,6 +1930,9 @@
       </c>
       <c r="AI15" t="n">
         <v>5</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="16">
@@ -1998,6 +2045,9 @@
       <c r="AI16" t="n">
         <v>5</v>
       </c>
+      <c r="AJ16" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2080,7 +2130,7 @@
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>test/data/stage</t>
+          <t>test/data/target</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
@@ -2109,6 +2159,9 @@
       <c r="AI17" t="n">
         <v>5</v>
       </c>
+      <c r="AJ17" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2228,6 +2281,9 @@
       <c r="AI18" t="n">
         <v>5</v>
       </c>
+      <c r="AJ18" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -2347,6 +2403,9 @@
       <c r="AI19" t="n">
         <v>5</v>
       </c>
+      <c r="AJ19" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -2469,6 +2528,9 @@
       </c>
       <c r="AI20" t="n">
         <v>8</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="21">
@@ -2589,6 +2651,9 @@
       <c r="AI21" t="n">
         <v>8</v>
       </c>
+      <c r="AJ21" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -2715,6 +2780,9 @@
       </c>
       <c r="AI22" t="n">
         <v>8</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="23">
@@ -2835,6 +2903,9 @@
       <c r="AI23" t="n">
         <v>5</v>
       </c>
+      <c r="AJ23" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2950,6 +3021,9 @@
       <c r="AI24" t="n">
         <v>8</v>
       </c>
+      <c r="AJ24" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2961,7 +3035,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -3060,6 +3134,9 @@
       </c>
       <c r="AI25" t="n">
         <v>8</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="26">
@@ -3180,6 +3257,9 @@
       <c r="AI26" t="n">
         <v>5</v>
       </c>
+      <c r="AJ26" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3302,6 +3382,9 @@
       </c>
       <c r="AI27" t="n">
         <v>8</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="28">
@@ -3378,6 +3461,9 @@
       <c r="AI28" t="n">
         <v>8</v>
       </c>
+      <c r="AJ28" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3497,6 +3583,9 @@
       <c r="AI29" t="n">
         <v>8</v>
       </c>
+      <c r="AJ29" t="n">
+        <v>1000</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -3615,6 +3704,9 @@
       </c>
       <c r="AI30" t="n">
         <v>8</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>1000</v>
       </c>
     </row>
     <row r="31">
@@ -3691,6 +3783,119 @@
       <c r="AI31" t="n">
         <v>8</v>
       </c>
+      <c r="AJ31" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>testcase31_snowflake_parquet_validation</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>likeobjectcompare</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Auto</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>rtpcr_source</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>raw_snowflake_sql_connection</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>snowflake</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>table</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>rtpcr_diagnostic_lab_testing</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>rtpcr_target</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>aws-s3</t>
+        </is>
+      </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>parquet</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>test/data/target</t>
+        </is>
+      </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>patients_target_parquet_mismatch</t>
+        </is>
+      </c>
+      <c r="Y32" t="inlineStr"/>
+      <c r="Z32" t="inlineStr"/>
+      <c r="AA32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr"/>
+      <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="inlineStr"/>
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>test/s2t/s2t_31_snowflake_parquet_val.xlsx</t>
+        </is>
+      </c>
+      <c r="AG32" t="inlineStr">
+        <is>
+          <t>source_to_target</t>
+        </is>
+      </c>
+      <c r="AH32" t="inlineStr">
+        <is>
+          <t>id,state</t>
+        </is>
+      </c>
+      <c r="AI32" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>2000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>